<commit_message>
Added in Elementalist doc 1 skills (big one)
</commit_message>
<xml_diff>
--- a/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
+++ b/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\5-Elementalist\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="1-Pillar" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil1 (3)" sheetId="3" r:id="rId3"/>
     <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="49">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -90,6 +90,96 @@
   </si>
   <si>
     <t>[[Number of turns between two casts: -  ]]</t>
+  </si>
+  <si>
+    <t>Pillar</t>
+  </si>
+  <si>
+    <t>Can only be summoned on empty cell.</t>
+  </si>
+  <si>
+    <t>When in Neutral state: The pillar get the element effect of the damage skill touching it (Only work for the Elementalist that summoned it) (00 turns)</t>
+  </si>
+  <si>
+    <t>Replicate the summoner skills whit the element effect of the pillar.</t>
+  </si>
+  <si>
+    <t>Unmovable.</t>
+  </si>
+  <si>
+    <t>When a player start his turn on the pillar glyph, +1lvl of the same element effect of the pillar.</t>
+  </si>
+  <si>
+    <t>When a player get damage by a skill replicated by the pillar, +1lvl of the same element effect of the pillar.</t>
+  </si>
+  <si>
+    <t>Fire Pillar</t>
+  </si>
+  <si>
+    <t>Water Pillar</t>
+  </si>
+  <si>
+    <t>Earth Pillar</t>
+  </si>
+  <si>
+    <t>Air Pillar</t>
+  </si>
+  <si>
+    <t>Pillar resistance: [[0% earth resistence, -50% fire resistence, 100% water resistence, 0% air resistence, 50% light resistence, 50% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Summon a ''Pillar'' [[50% summoner HP, 0 AP, 0 MP, 0% earth resistence, 0% fire resistence, 0% water resistence, 0% air resistence, 50% light resistence, 50% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Water''. [[Max effect accumulation: 5 ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>Pillar resistance: [[100% earth resistence, 0% fire resistence, 100% water resistence, -50% air resistence, 50% light resistence, 50% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Earth''. [[Max effect accumulation: 5 ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>Pillar resistance: [[0% earth resistence, 100% fire resistence, -50% water resistence, 0% air resistence, 50% light resistence, 50% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Fire''. [[Max effect accumulation: 5 ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>Pillar resistance: [[-50% earth resistence, 0% fire resistence, 0% water resistence, 100% air resistence, 50% light resistence, 50% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Air''. [[Max effect accumulation: 5 ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>[[AP: 5 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1-3 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Line of sight: No ]]</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: No ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Circle whit 2 cells radius ]] (Elemental Glyph)</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 5  ]]</t>
+  </si>
+  <si>
+    <t>Only the summoner is not affected by the replicated skills.</t>
+  </si>
+  <si>
+    <t>The mainstay of my abilities! which way i'll use it?</t>
+  </si>
+  <si>
+    <t>Pillar: Effect name: ''Neutral''.</t>
   </si>
 </sst>
 </file>
@@ -155,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -172,11 +262,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -199,6 +330,25 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +687,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -549,66 +699,64 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -620,108 +768,229 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="1"/>
+      <c r="C27" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
+      <c r="C29" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
+      <c r="C31" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
+      <c r="D32" s="16"/>
+    </row>
+    <row r="33" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="1"/>
+      <c r="C35" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="1"/>
+      <c r="C36" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B38" s="1"/>
+      <c r="C38" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="1"/>
+      <c r="C40" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="1"/>
+      <c r="C41" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B43" s="1"/>
+      <c r="C43" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="1"/>
+      <c r="C45" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="1"/>
+      <c r="C46" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B48" s="1"/>
+      <c r="C48" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="1"/>
+      <c r="C50" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="1"/>
+      <c r="C51" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 1 skill in Elementalist doc. Also added interresting information about 2D character creation tool and more.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
+++ b/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-Pillar" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="2-CorrosiveRain" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil1 (3)" sheetId="3" r:id="rId3"/>
     <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
     <sheet name="Feuil1 (5)" sheetId="5" r:id="rId5"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="59">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -180,6 +180,36 @@
   </si>
   <si>
     <t>Pillar: Effect name: ''Neutral''.</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - On each line at 2 and 4 cell of range ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 0 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: No ]]</t>
+  </si>
+  <si>
+    <t>[[AP: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  20-40 water ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 2 ]]</t>
+  </si>
+  <si>
+    <t>Other: [[Reduce resistance by 5%]] (1 turn)</t>
+  </si>
+  <si>
+    <t>A slightly corrosive rain to ruin the armour pieces.</t>
+  </si>
+  <si>
+    <t>Corrosive Rain</t>
+  </si>
+  <si>
+    <t>Effect name: ''Corrosive Rain''.</t>
   </si>
 </sst>
 </file>
@@ -666,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -1217,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1270,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1252,40 +1282,38 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1297,134 +1325,75 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1437,7 +1406,7 @@
   <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added 3 skills in Elementalist doc. Also redefined the skills description standard, need to modifie the previously done class skills description.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
+++ b/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1-Pillar" sheetId="1" r:id="rId1"/>
     <sheet name="2-CorrosiveRain" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil1 (3)" sheetId="3" r:id="rId3"/>
-    <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
-    <sheet name="Feuil1 (5)" sheetId="5" r:id="rId5"/>
+    <sheet name="3-WindWave" sheetId="3" r:id="rId3"/>
+    <sheet name="4-RisingGround" sheetId="4" r:id="rId4"/>
+    <sheet name="5-FireBeam" sheetId="5" r:id="rId5"/>
     <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
     <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
     <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="83">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Pillar resistance: [[0% earth resistence, -50% fire resistence, 100% water resistence, 0% air resistence, 50% light resistence, 50% dark resistence]]</t>
   </si>
   <si>
-    <t>Summon a ''Pillar'' [[50% summoner HP, 0 AP, 0 MP, 0% earth resistence, 0% fire resistence, 0% water resistence, 0% air resistence, 50% light resistence, 50% dark resistence]]</t>
-  </si>
-  <si>
     <t>Effect name: ''Water''. [[Max effect accumulation: 5 ]] (00 turns)</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>Only the summoner is not affected by the replicated skills.</t>
   </si>
   <si>
-    <t>The mainstay of my abilities! which way i'll use it?</t>
-  </si>
-  <si>
     <t>Pillar: Effect name: ''Neutral''.</t>
   </si>
   <si>
@@ -194,22 +188,100 @@
     <t>[[AP: 3 ]]</t>
   </si>
   <si>
-    <t>[[Damage:  20-40 water ]]</t>
-  </si>
-  <si>
     <t>[[Number of casts per turn: 2 ]]</t>
   </si>
   <si>
-    <t>Other: [[Reduce resistance by 5%]] (1 turn)</t>
-  </si>
-  <si>
-    <t>A slightly corrosive rain to ruin the armour pieces.</t>
-  </si>
-  <si>
     <t>Corrosive Rain</t>
   </si>
   <si>
     <t>Effect name: ''Corrosive Rain''.</t>
+  </si>
+  <si>
+    <t>Wind Wave</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Hollow circle at 2 cells radius ]]</t>
+  </si>
+  <si>
+    <t>[[AP: 4 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  20-30 water ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  25-35 air ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Wind Wave''.</t>
+  </si>
+  <si>
+    <t>[[Reduce dealt damage by 5%]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Inflicts Air-type damage and reduces the</t>
+  </si>
+  <si>
+    <t>[[Reduce resistance by 3%]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Self: Isn't affected by the mimic of this skill from the ''Pillar''.</t>
+  </si>
+  <si>
+    <t>dealt damage in the area of effect.</t>
+  </si>
+  <si>
+    <t>Inflicts Water-type damage and reduces</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> resistance in the area of effect.</t>
+  </si>
+  <si>
+    <t>Summons a Pillar that need to be hit whit the Elementalist skills to set his element states. The pillar replicate the Elementalist skills and convert the element-type into the pillar type when hit. The glyph under the Pillar give effect used by other Elementalist skills.</t>
+  </si>
+  <si>
+    <t>Rising Ground</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - On each diagonal line at 1 and 2 diagonal cells of range ]]</t>
+  </si>
+  <si>
+    <t>Summons only on empty cell.</t>
+  </si>
+  <si>
+    <t>Summons a ''Stalagmite'' [[5% summoner HP, 0 AP, 0 MP, 75% earth resistence, 75% fire resistence, -25% water resistence, 75% air resistence, 50% light resistence, 50% dark resistence]] (1 turn)</t>
+  </si>
+  <si>
+    <t>[[MP: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  25-35 earh ]]</t>
+  </si>
+  <si>
+    <t>Summons a ''Pillar'' [[50% summoner HP, 0 AP, 0 MP, 0% earth resistence, 0% fire resistence, 0% water resistence, 0% air resistence, 50% light resistence, 50% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage and summons Stalagmite on empty cells in the area of effect.</t>
+  </si>
+  <si>
+    <t>Fire Beam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Area of effect: - Straight line of cells ]] (Modular area) </t>
+  </si>
+  <si>
+    <t>[[Damage:  50-60 fire - ((range casted - 1) * 3) ]]</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: Yes ]]</t>
+  </si>
+  <si>
+    <t>All the cells between the targetted cell and the Elementalist are part of the area of effect.</t>
+  </si>
+  <si>
+    <t>Inflicts Fire-type damage in a modular area of effect. The farthest it's used, the less damage is dealt.</t>
   </si>
 </sst>
 </file>
@@ -337,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -379,6 +451,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -726,10 +817,10 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>47</v>
+      <c r="C5" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -741,14 +832,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -760,21 +851,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -786,7 +877,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -798,7 +889,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -810,14 +901,14 @@
     <row r="18" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="12" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -889,7 +980,7 @@
     <row r="31" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B31" s="1"/>
       <c r="C31" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="1"/>
     </row>
@@ -920,7 +1011,7 @@
     <row r="36" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B36" s="1"/>
       <c r="C36" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -944,14 +1035,14 @@
     <row r="40" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B40" s="1"/>
       <c r="C40" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B41" s="1"/>
       <c r="C41" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41" s="1"/>
     </row>
@@ -975,14 +1066,14 @@
     <row r="45" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B45" s="1"/>
       <c r="C45" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B46" s="1"/>
       <c r="C46" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D46" s="1"/>
     </row>
@@ -1006,14 +1097,14 @@
     <row r="50" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B50" s="1"/>
       <c r="C50" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B51" s="1"/>
       <c r="C51" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D51" s="1"/>
     </row>
@@ -1247,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1361,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1282,20 +1373,20 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
@@ -1307,93 +1398,107 @@
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="1"/>
+      <c r="C17" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="1"/>
+      <c r="C18" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B21" s="1"/>
-      <c r="C21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B23" s="1"/>
-      <c r="C23" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="1"/>
+      <c r="C25" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1403,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1531,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1438,14 +1543,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1457,160 +1562,113 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="21" t="s">
+        <v>61</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1620,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,7 +1701,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1652,182 +1710,135 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="22" t="s">
+        <v>72</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1837,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,7 +1871,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1869,69 +1880,67 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1943,45 +1952,37 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1990,61 +1991,17 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="24" t="s">
+        <v>81</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified all the skills descriptions in the guardian doc to match the new standard.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
+++ b/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-Pillar" sheetId="1" r:id="rId1"/>
@@ -263,9 +263,6 @@
     <t>Summons a ''Pillar'' [[50% summoner HP, 0 AP, 0 MP, 0% earth resistence, 0% fire resistence, 0% water resistence, 0% air resistence, 50% light resistence, 50% dark resistence]]</t>
   </si>
   <si>
-    <t>Inflicts Earth-type damage and summons Stalagmite on empty cells in the area of effect.</t>
-  </si>
-  <si>
     <t>Fire Beam</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>Inflicts Fire-type damage in a modular area of effect. The farthest it's used, the less damage is dealt.</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage and summons Stalagmite on the empty cells in the area of effect.</t>
   </si>
 </sst>
 </file>
@@ -1340,7 +1340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1681,7 +1681,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,7 +1713,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="23" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1850,7 +1850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -1871,7 +1871,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1883,7 +1883,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1928,7 +1928,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1952,7 +1952,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1964,7 +1964,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1994,7 +1994,7 @@
     <row r="24" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="1"/>
     </row>

</xml_diff>

<commit_message>
upgraded the doc of the Elementalist.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
+++ b/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1-Pillar" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="73">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -95,24 +95,6 @@
     <t>Pillar</t>
   </si>
   <si>
-    <t>Can only be summoned on empty cell.</t>
-  </si>
-  <si>
-    <t>When in Neutral state: The pillar get the element effect of the damage skill touching it (Only work for the Elementalist that summoned it) (00 turns)</t>
-  </si>
-  <si>
-    <t>Replicate the summoner skills whit the element effect of the pillar.</t>
-  </si>
-  <si>
-    <t>Unmovable.</t>
-  </si>
-  <si>
-    <t>When a player start his turn on the pillar glyph, +1lvl of the same element effect of the pillar.</t>
-  </si>
-  <si>
-    <t>When a player get damage by a skill replicated by the pillar, +1lvl of the same element effect of the pillar.</t>
-  </si>
-  <si>
     <t>Fire Pillar</t>
   </si>
   <si>
@@ -170,9 +152,6 @@
     <t>[[Number of turns between two casts: 5  ]]</t>
   </si>
   <si>
-    <t>Only the summoner is not affected by the replicated skills.</t>
-  </si>
-  <si>
     <t>Pillar: Effect name: ''Neutral''.</t>
   </si>
   <si>
@@ -227,9 +206,6 @@
     <t>[[Reduce resistance by 3%]] (1 turn)</t>
   </si>
   <si>
-    <t>Self: Isn't affected by the mimic of this skill from the ''Pillar''.</t>
-  </si>
-  <si>
     <t>dealt damage in the area of effect.</t>
   </si>
   <si>
@@ -239,18 +215,12 @@
     <t xml:space="preserve"> resistance in the area of effect.</t>
   </si>
   <si>
-    <t>Summons a Pillar that need to be hit whit the Elementalist skills to set his element states. The pillar replicate the Elementalist skills and convert the element-type into the pillar type when hit. The glyph under the Pillar give effect used by other Elementalist skills.</t>
-  </si>
-  <si>
     <t>Rising Ground</t>
   </si>
   <si>
     <t>[[Area of effect: - On each diagonal line at 1 and 2 diagonal cells of range ]]</t>
   </si>
   <si>
-    <t>Summons only on empty cell.</t>
-  </si>
-  <si>
     <t>Summons a ''Stalagmite'' [[5% summoner HP, 0 AP, 0 MP, 75% earth resistence, 75% fire resistence, -25% water resistence, 75% air resistence, 50% light resistence, 50% dark resistence]] (1 turn)</t>
   </si>
   <si>
@@ -275,13 +245,13 @@
     <t>[[Cast in straight line: Yes ]]</t>
   </si>
   <si>
-    <t>All the cells between the targetted cell and the Elementalist are part of the area of effect.</t>
-  </si>
-  <si>
-    <t>Inflicts Fire-type damage in a modular area of effect. The farthest it's used, the less damage is dealt.</t>
-  </si>
-  <si>
-    <t>Inflicts Earth-type damage and summons Stalagmite on the empty cells in the area of effect.</t>
+    <t>Summons an unmovable Pillar on an empty cell that need to be hit whit the Elementalist skills to set his element states.                                                                 The pillar replicate the Elementalist skills and convert the element-type into the pillar type when hit and give elemental effect to damaged entity.                                                                            The caster is not affected by the replication of the skills.                                                                The glyph under the Pillar give elemental effect used by other Elementalist skills.</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage and summons Stalagmite on the empty cells for the current turn in the area of effect.</t>
+  </si>
+  <si>
+    <t>Inflicts Fire-type damage in a modular area of effect.                      All the cells between the targetted cell and the caster are part of the area of effect.                                                                                   The farthest it's used, the less damage is dealt.</t>
   </si>
 </sst>
 </file>
@@ -347,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -392,24 +362,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -442,16 +399,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -470,6 +418,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,9 +736,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D52"/>
+  <dimension ref="B2:D46"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -817,10 +768,10 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="156" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="19" t="s">
-        <v>68</v>
+      <c r="C5" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -832,14 +783,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -851,21 +802,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -877,7 +828,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -889,7 +840,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -900,15 +851,15 @@
     </row>
     <row r="18" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="12" t="s">
-        <v>75</v>
+      <c r="C18" s="22" t="s">
+        <v>65</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="17" t="s">
-        <v>46</v>
+      <c r="C19" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -937,181 +888,137 @@
     </row>
     <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="C25" s="11"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
-      <c r="C26" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C26" s="1"/>
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
-      <c r="C27" s="14" t="s">
-        <v>23</v>
+      <c r="C27" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
-      <c r="C28" s="11" t="s">
-        <v>24</v>
-      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
       <c r="C29" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B30" s="1"/>
       <c r="C30" s="11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
-      <c r="C31" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="16"/>
-    </row>
-    <row r="33" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
-      <c r="C33" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="C34" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B35" s="1"/>
       <c r="C35" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
-      <c r="C36" s="11" t="s">
-        <v>31</v>
-      </c>
+      <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="C37" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="1"/>
+      <c r="C39" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B40" s="1"/>
       <c r="C40" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
-      <c r="C41" s="11" t="s">
-        <v>33</v>
-      </c>
+      <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="C42" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
-      <c r="C43" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="C44" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B45" s="1"/>
       <c r="C45" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
-      <c r="C46" s="11" t="s">
-        <v>35</v>
-      </c>
+      <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B48" s="1"/>
-      <c r="C48" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="1"/>
-      <c r="C50" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D50" s="1"/>
-    </row>
-    <row r="51" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="1"/>
-      <c r="C51" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1338,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,7 +1268,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1373,14 +1280,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1392,14 +1299,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1411,7 +1318,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1423,7 +1330,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1435,7 +1342,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1446,15 +1353,15 @@
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="21" t="s">
-        <v>58</v>
+      <c r="C17" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="21" t="s">
-        <v>63</v>
+      <c r="C18" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1484,21 +1391,14 @@
     <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="13" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="16"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1507,346 +1407,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="1"/>
-      <c r="C17" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="1"/>
-      <c r="C18" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="1"/>
-      <c r="C24" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="1"/>
-      <c r="C25" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="39" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="1"/>
-      <c r="C17" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="C18" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="1"/>
-      <c r="C24" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="1"/>
-      <c r="C25" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D25"/>
   <sheetViews>
@@ -1871,7 +1431,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1880,91 +1440,91 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="18" t="s">
-        <v>81</v>
+      <c r="C5" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="18" t="s">
+        <v>52</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>78</v>
+      <c r="C18" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1986,22 +1546,344 @@
       </c>
       <c r="D22" s="1"/>
     </row>
+    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D25"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="1"/>
+      <c r="C17" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="24" t="s">
-        <v>80</v>
-      </c>
+      <c r="C24" s="21"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="16"/>
+      <c r="D25" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added in the doc 3 Elementalist skills.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
+++ b/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1-Pillar" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
     <sheet name="3-WindWave" sheetId="3" r:id="rId3"/>
     <sheet name="4-RisingGround" sheetId="4" r:id="rId4"/>
     <sheet name="5-FireBeam" sheetId="5" r:id="rId5"/>
-    <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
-    <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
-    <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
+    <sheet name="6-Teleportation " sheetId="6" r:id="rId6"/>
+    <sheet name="7-MagicBarrier" sheetId="7" r:id="rId7"/>
+    <sheet name="8-ElementalImmunity" sheetId="8" r:id="rId8"/>
     <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
     <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
   </sheets>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -252,6 +252,78 @@
   </si>
   <si>
     <t>Inflicts Fire-type damage in a modular area of effect.                      All the cells between the targetted cell and the caster are part of the area of effect.                                                                                   The farthest it's used, the less damage is dealt.</t>
+  </si>
+  <si>
+    <t>[[Range: 2-4 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 4 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell]]</t>
+  </si>
+  <si>
+    <t>Teleport the player at the targeted cell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Teleports to the targeted cell.</t>
+  </si>
+  <si>
+    <t>Teleportation </t>
+  </si>
+  <si>
+    <t>Magic Barrier</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 6 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Hollow square of 2 cells radius]]</t>
+  </si>
+  <si>
+    <t>The glyphs prevent the cells to be walked over.                               The "Pillar" also reproduce the glyph pattern.</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Line of sight: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 0-2 ]]</t>
+  </si>
+  <si>
+    <t>[[MP: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[AP: 1 ]]</t>
+  </si>
+  <si>
+    <t>Protect the caster to elementals-type damage but weaken it from dark and light damage.                                                                              OR                                                                                                          Protect the target from the damage dealt by the caster skills and his "Pillar".</t>
+  </si>
+  <si>
+    <t>Elemental Immunity</t>
+  </si>
+  <si>
+    <t>Effect name: ''Elemental Immunity''.</t>
+  </si>
+  <si>
+    <t>Glyph (1 turn)</t>
+  </si>
+  <si>
+    <t>Other target: Immunity from the Elementalist skills and his "Pillar" (1 turn)</t>
+  </si>
+  <si>
+    <t>Self targeting: [[Boost water, air, earth and fire resistance by 50%]]    (1 turn)</t>
+  </si>
+  <si>
+    <t>Self targeting:  [[Reduce dark and light resistance by 100%]]          (1 turn)</t>
   </si>
 </sst>
 </file>
@@ -317,7 +389,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -362,11 +434,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -420,6 +505,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -738,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -1734,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,10 +1981,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,7 +2004,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1928,179 +2016,130 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="10"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2110,10 +2149,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2172,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2142,182 +2181,119 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="16" t="s">
+        <v>83</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2327,10 +2303,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2350,7 +2326,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2359,119 +2335,121 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="C16" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+    <row r="20" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+      <c r="B20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="23" t="s">
+        <v>96</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2480,61 +2458,35 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 1 skill in Elementalist doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
+++ b/GameDesign/Class/5-Elementalist/Documentation/ElementalistSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-Pillar" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="6-Teleportation " sheetId="6" r:id="rId6"/>
     <sheet name="7-MagicBarrier" sheetId="7" r:id="rId7"/>
     <sheet name="8-ElementalImmunity" sheetId="8" r:id="rId8"/>
-    <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
-    <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
+    <sheet name="9-ElementalBackfire" sheetId="9" r:id="rId9"/>
+    <sheet name="Feuil1 (10)" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="109">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -324,6 +324,42 @@
   </si>
   <si>
     <t>Self targeting:  [[Reduce dark and light resistance by 100%]]          (1 turn)</t>
+  </si>
+  <si>
+    <t>Elemental Backfire</t>
+  </si>
+  <si>
+    <t>Effect name: ''Earth''.  [[Max effect accumulation: 5 ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Fire''.    [[Max effect accumulation: 5 ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Air''.      [[Max effect accumulation: 5 ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20% chance: [[ - ]] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">increase an random element effect of an entity dealing damage to the target of this skill.  </t>
+  </si>
+  <si>
+    <t>20% chance: [[ +1 ''Water'' effect ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>20% chance: [[ +1 ''Earth'' effect ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>20% chance: [[ +1 ''Fire'' effect ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>20% chance: [[ +1 ''Air'' effect ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>[[AP: 2 ]]</t>
   </si>
 </sst>
 </file>
@@ -827,7 +863,7 @@
   <dimension ref="B2:D46"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,8 +2341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2499,7 +2535,7 @@
   <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2519,7 +2555,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2528,175 +2564,177 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
+    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B27" s="1"/>
+      <c r="C27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
+      <c r="C29" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
       <c r="C31" s="10" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B32" s="1"/>
       <c r="C32" s="10" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>